<commit_message>
Updated Notebook and outputs
</commit_message>
<xml_diff>
--- a/Clean Order Data.xlsx
+++ b/Clean Order Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,40 +471,35 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Order Name</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Surname</t>
+          <t>Order Email</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Order Email</t>
+          <t>Street</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Street</t>
+          <t>Mail Box</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Box</t>
+          <t>County</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>Country</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Country</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Mail Code</t>
         </is>
@@ -542,40 +537,35 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Dana</t>
+          <t>Dana Nguyen</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Nguyen</t>
+          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -613,40 +603,35 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Dana</t>
+          <t>Dana Nguyen</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Nguyen</t>
+          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -684,40 +669,35 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Dana</t>
+          <t>Dana Nguyen</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Nguyen</t>
+          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -755,40 +735,35 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Cheryl</t>
+          <t>Cheryl Bradley</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Bradley</t>
+          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -826,40 +801,35 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Dana</t>
+          <t>Dana Nguyen</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Nguyen</t>
+          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -897,40 +867,35 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Cheryl</t>
+          <t>Cheryl Bradley</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Bradley</t>
+          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -968,40 +933,35 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cheryl</t>
+          <t>Cheryl Bradley</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Bradley</t>
+          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -1039,40 +999,35 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Dana</t>
+          <t>Dana Nguyen</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Nguyen</t>
+          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -1110,40 +1065,35 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Dana</t>
+          <t>Dana Nguyen</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Nguyen</t>
+          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>DANA.NGUYEN@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -1181,40 +1131,35 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cheryl</t>
+          <t>Cheryl Bradley</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Bradley</t>
+          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -1252,40 +1197,35 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cheryl</t>
+          <t>Cheryl Bradley</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Bradley</t>
+          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>CHERYL.BRADLEY@CUSTOMER-1.COM</t>
+          <t>PSC 4115</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>PSC 4115</t>
+          <t>Box 7815</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Box 7815</t>
+          <t>APO</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
         <is>
           <t>AA 41945</t>
         </is>
@@ -1323,40 +1263,35 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Tasha</t>
+          <t>Tasha Rodriguez</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1394,40 +1329,35 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Tasha</t>
+          <t>Tasha Rodriguez</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1465,40 +1395,35 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Bobby</t>
+          <t>Bobby Flores</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1536,40 +1461,35 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Walter</t>
+          <t>Walter Pratt</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Pratt</t>
+          <t>WALTER.PRATT@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>WALTER.PRATT@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1607,40 +1527,35 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Tasha</t>
+          <t>Tasha Rodriguez</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1678,40 +1593,35 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Tasha</t>
+          <t>Tasha Rodriguez</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1749,40 +1659,35 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Bobby</t>
+          <t>Bobby Flores</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1820,40 +1725,35 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Tasha</t>
+          <t>Tasha Rodriguez</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>TASHA.RODRIGUEZ@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1891,40 +1791,35 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Bobby</t>
+          <t>Bobby Flores</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -1962,40 +1857,35 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Walter</t>
+          <t>Walter Pratt</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Pratt</t>
+          <t>WALTER.PRATT@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>WALTER.PRATT@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -2033,40 +1923,35 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Bobby</t>
+          <t>Bobby Flores</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -2104,40 +1989,35 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Bobby</t>
+          <t>Bobby Flores</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>BOBBY.FLORES@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -2175,40 +2055,35 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-2.COM</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-2.COM</t>
+          <t>778 Brown Plaza</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>778 Brown Plaza</t>
+          <t>Box 985</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Box 985</t>
+          <t>North Jenniferfurt</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>North Jenniferfurt</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
         <is>
           <t>VT 88077</t>
         </is>
@@ -2246,40 +2121,35 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2317,40 +2187,35 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Michelle Kelley</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Kelley</t>
+          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2388,40 +2253,35 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Michelle Kelley</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Kelley</t>
+          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2459,40 +2319,35 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2530,40 +2385,35 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O30" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2601,40 +2451,35 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Michelle Kelley</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Kelley</t>
+          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O31" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2672,40 +2517,35 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O32" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2743,40 +2583,35 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Michelle Kelley</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Kelley</t>
+          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O33" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2814,40 +2649,35 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O34" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2885,40 +2715,35 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O35" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -2956,40 +2781,35 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O36" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -3027,40 +2847,35 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O37" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -3098,40 +2913,35 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Michelle Kelley</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Kelley</t>
+          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O38" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -3169,40 +2979,35 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Kimberly</t>
+          <t>Kimberly Maynard</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Maynard</t>
+          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>KIMBERLY.MAYNARD@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O39" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -3240,40 +3045,35 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Michelle Kelley</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Kelley</t>
+          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>MICHELLE.KELLEY@CUSTOMER-3.COM</t>
+          <t>3513 John Divide Suite</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>3513 John Divide Suite</t>
+          <t>Box 115</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Box 115</t>
+          <t>Rodriguezside</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Rodriguezside</t>
+          <t>England</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
         <is>
           <t>LA 93111</t>
         </is>
@@ -3311,40 +3111,35 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Mary Alvarez</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Alvarez</t>
+          <t>MARY.ALVAREZ@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>MARY.ALVAREZ@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3382,40 +3177,35 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Laurie</t>
+          <t>Laurie Wallace</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Wallace</t>
+          <t>LAURIE.WALLACE@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>LAURIE.WALLACE@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3453,40 +3243,35 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Collin</t>
+          <t>Collin Lopez</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Lopez</t>
+          <t>COLLIN.LOPEZ@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>COLLIN.LOPEZ@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3524,40 +3309,35 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Collin</t>
+          <t>Collin Lopez</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Lopez</t>
+          <t>COLLIN.LOPEZ@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>COLLIN.LOPEZ@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3595,40 +3375,35 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Mary Alvarez</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Alvarez</t>
+          <t>MARY.ALVAREZ@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>MARY.ALVAREZ@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3666,40 +3441,35 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Mary Alvarez</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Alvarez</t>
+          <t>MARY.ALVAREZ@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>MARY.ALVAREZ@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O46" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3737,40 +3507,35 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Mary Alvarez</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Alvarez</t>
+          <t>MARY.ALVAREZ@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>MARY.ALVAREZ@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O47" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3808,40 +3573,35 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Laurie</t>
+          <t>Laurie Wallace</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Wallace</t>
+          <t>LAURIE.WALLACE@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>LAURIE.WALLACE@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O48" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3879,40 +3639,35 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Laurie</t>
+          <t>Laurie Wallace</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Wallace</t>
+          <t>LAURIE.WALLACE@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>LAURIE.WALLACE@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O49" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -3950,40 +3705,35 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Janice</t>
+          <t>Janice Johnston</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Johnston</t>
+          <t>JANICE.JOHNSTON@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>JANICE.JOHNSTON@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O50" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>
@@ -4021,40 +3771,35 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Collin</t>
+          <t>Collin Lopez</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Lopez</t>
+          <t>COLLIN.LOPEZ@CUSTOMER-4.COM</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>COLLIN.LOPEZ@CUSTOMER-4.COM</t>
+          <t xml:space="preserve">398 Wallace Ranch </t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t xml:space="preserve">398 Wallace Ranch </t>
+          <t>Suite 593</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Suite 593</t>
+          <t>Ivanburgh</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Ivanburgh</t>
+          <t>Usa</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
-        <is>
-          <t>Usa</t>
-        </is>
-      </c>
-      <c r="O51" t="inlineStr">
         <is>
           <t>AZ 80818</t>
         </is>

</xml_diff>